<commit_message>
Add comprehensive progress display system and UNC access enhancements
- Progress Display System: Configurable bar/verbose modes with timestamps
- UNC Access Improvements: Data preservation on failures, counter consistency
- Enhanced Error Handling: Preserve existing data when UNC access fails
- Documentation Updates: Complete refresh of README.md, CLAUDE.md, implementation.md
- Build System: Dependency management and JAVA_HOME support enhancements

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533EA3D0-82D9-4DCA-9554-5AD1E809B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D956858-6D80-4CCF-9BA0-51476B36D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{57A338DE-0F7B-47ED-A2B0-7733E1C8763A}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -84,34 +84,43 @@
     <t>JarVersion</t>
   </si>
   <si>
+    <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\poi-5.4.1.jar</t>
+  </si>
+  <si>
+    <t>ScanError</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>Windows_2019</t>
+  </si>
+  <si>
+    <t>NOTPRIME2</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>2025-08-24 17:59:48</t>
+  </si>
+  <si>
     <t>2.20.0</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2025-08-24 17:59:48</t>
-  </si>
-  <si>
-    <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\poi-5.4.1.jar</t>
+    <t/>
+  </si>
+  <si>
+    <t>UNC access denied - cannot determine file existence</t>
   </si>
   <si>
     <t>2025-08-23 22:39:06</t>
   </si>
   <si>
     <t>5.4.1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ScanError</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>dd</t>
   </si>
 </sst>
 </file>
@@ -484,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152CCE6C-5592-430F-AB5A-C8E106F002E5}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,6 +507,7 @@
     <col min="4" max="4" customWidth="true" width="16.54296875"/>
     <col min="6" max="6" customWidth="true" width="36.26953125"/>
     <col min="7" max="7" customWidth="true" width="11.0"/>
+    <col min="8" max="8" customWidth="true" width="46.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -523,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -540,16 +550,16 @@
         <v>9</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -557,13 +567,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>9</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -571,25 +584,42 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>19</v>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -611,12 +641,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RemoteScanError column and dual logging functionality
- Add RemoteScanError column for remote UNC access errors
- Separate local (ScanError) from remote (RemoteScanError) error handling
- Clear error columns for successful scans (local and remote)
- Add dual logging to console and optional log file
- Remove progress.display setting - always use timestamped logging
- Update UNC timeout from 30 to 7 seconds
- Update documentation for new error handling and logging

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D956858-6D80-4CCF-9BA0-51476B36D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67959484-6B78-40D9-9C9F-7B9DC435BF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{57A338DE-0F7B-47ED-A2B0-7733E1C8763A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -19,22 +19,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Export!$A$1:$G$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -43,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -54,40 +40,49 @@
     <t>XTRACT_PATH</t>
   </si>
   <si>
+    <t>OTHER_COLUMN</t>
+  </si>
+  <si>
+    <t>FileExists</t>
+  </si>
+  <si>
+    <t>FileModificationDate</t>
+  </si>
+  <si>
+    <t>JarVersion</t>
+  </si>
+  <si>
+    <t>ScanError</t>
+  </si>
+  <si>
     <t>LPRIME</t>
   </si>
   <si>
+    <t>Windows-2019</t>
+  </si>
+  <si>
+    <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\commons-io-2.20.0.jar</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>NOTPRIME</t>
   </si>
   <si>
-    <t>Windows-2019</t>
+    <t>Windows_2019</t>
   </si>
   <si>
     <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\commons-collections4-4.5.0.jar</t>
   </si>
   <si>
-    <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\commons-io-2.20.0.jar</t>
-  </si>
-  <si>
-    <t>OTHER_COLUMN</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>FileExists</t>
-  </si>
-  <si>
-    <t>FileModificationDate</t>
-  </si>
-  <si>
-    <t>JarVersion</t>
+    <t>Windows Server 2019</t>
   </si>
   <si>
     <t>D:\Docs\Projects\Code\VulnAnalysisTool\deps\poi-5.4.1.jar</t>
   </si>
   <si>
-    <t>ScanError</t>
+    <t>NOTPRIME2</t>
   </si>
   <si>
     <t>DD</t>
@@ -96,10 +91,7 @@
     <t>dd</t>
   </si>
   <si>
-    <t>Windows_2019</t>
-  </si>
-  <si>
-    <t>NOTPRIME2</t>
+    <t>RemoteScanError</t>
   </si>
   <si>
     <t>Y</t>
@@ -114,13 +106,13 @@
     <t/>
   </si>
   <si>
+    <t>2025-08-23 22:39:06</t>
+  </si>
+  <si>
+    <t>5.4.1</t>
+  </si>
+  <si>
     <t>UNC access denied - cannot determine file existence</t>
-  </si>
-  <si>
-    <t>2025-08-23 22:39:06</t>
-  </si>
-  <si>
-    <t>5.4.1</t>
   </si>
 </sst>
 </file>
@@ -492,11 +484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152CCE6C-5592-430F-AB5A-C8E106F002E5}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H5"/>
+      <selection activeCell="E2" sqref="E2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,7 +502,7 @@
     <col min="8" max="8" customWidth="true" width="46.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -521,116 +513,116 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="B2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="E2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="B3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>14</v>
       </c>
+      <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s" s="0">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>22</v>
+      <c r="F4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s" s="0">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
-        <v>18</v>
-      </c>
       <c r="B5" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G4" xr:uid="{152CCE6C-5592-430F-AB5A-C8E106F002E5}"/>
+  <autoFilter ref="A1:G4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794B7212-7DD9-4576-934C-297BF18122AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -641,12 +633,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve code quality with standardized error handling and cleanup
- Add standardized error handling methods (recordScanError, recordRemoteScanError, addHostToExclusionList)
- Add helper methods to reduce code duplication (setFileNotFound, normalizeHostname, clearScanErrors)
- Remove unused imports (AtomicBoolean) and methods (setFileFound)
- Improve code consistency and maintainability while preserving functionality
- Update documentation to reflect code quality improvements

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67959484-6B78-40D9-9C9F-7B9DC435BF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E858950-5FBB-4520-B40F-BABF3A79BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -488,7 +488,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:I5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add ScanDate column to track when scans are performed
- Add ScanDate column that records timestamp when hostname is processed
- Auto-create ScanDate column alongside other output columns
- Record scan timestamp for all processed hosts (local and remote)
- Skip timestamp recording only for hostname mismatches
- Use consistent timestamp format matching other date fields

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>UNC access denied - cannot determine file existence</t>
+  </si>
+  <si>
+    <t>ScanDate</t>
+  </si>
+  <si>
+    <t>2025-09-09 08:23:02</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -530,6 +536,9 @@
       <c r="I1" t="s" s="0">
         <v>20</v>
       </c>
+      <c r="J1" t="s" s="0">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
@@ -556,6 +565,9 @@
       <c r="H2" t="s" s="0">
         <v>24</v>
       </c>
+      <c r="J2" t="s" s="0">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
@@ -596,6 +608,9 @@
       <c r="H4" t="s" s="0">
         <v>24</v>
       </c>
+      <c r="J4" t="s" s="0">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
@@ -612,6 +627,9 @@
       </c>
       <c r="I5" t="s" s="0">
         <v>27</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor invalid path detection and fix ScanDate to session timestamp
- Simplify checkForInvalidPath method to return boolean instead of InvalidPathResult object
- Remove unused InvalidPathResult class entirely
- Fix Windows platform detection to use actual platform column data (isWindowsPlatform) instead of path parsing
- Change ScanDate column to use single session timestamp for all rows instead of individual processing times
- Update documentation to reflect ScanDate represents session start time

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E858950-5FBB-4520-B40F-BABF3A79BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266B51A-63CA-4DF1-A2C1-0113B0BAA44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -94,6 +94,24 @@
     <t>RemoteScanError</t>
   </si>
   <si>
+    <t>ScanDate</t>
+  </si>
+  <si>
+    <t>D:\Docs\Projects\Code\VulnAnalysisTool\</t>
+  </si>
+  <si>
+    <t>N\A</t>
+  </si>
+  <si>
+    <t>2025-09-09 21:04:44</t>
+  </si>
+  <si>
+    <t>2025-09-09 21:04:49</t>
+  </si>
+  <si>
+    <t>2025-09-09 21:40:41</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -106,6 +124,9 @@
     <t/>
   </si>
   <si>
+    <t>2025-09-09 21:40:42</t>
+  </si>
+  <si>
     <t>2025-08-23 22:39:06</t>
   </si>
   <si>
@@ -115,10 +136,7 @@
     <t>UNC access denied - cannot determine file existence</t>
   </si>
   <si>
-    <t>ScanDate</t>
-  </si>
-  <si>
-    <t>2025-09-09 08:23:02</t>
+    <t>2025-09-09 21:40:47</t>
   </si>
 </sst>
 </file>
@@ -491,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,12 +521,12 @@
     <col min="2" max="2" customWidth="true" width="22.08984375"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="66.26953125"/>
     <col min="4" max="4" customWidth="true" width="16.54296875"/>
-    <col min="6" max="6" customWidth="true" width="36.26953125"/>
+    <col min="6" max="6" customWidth="true" width="20.7265625"/>
     <col min="7" max="7" customWidth="true" width="11.0"/>
-    <col min="8" max="8" customWidth="true" width="46.1796875"/>
+    <col min="8" max="8" customWidth="true" width="17.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -537,10 +555,10 @@
         <v>20</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
@@ -554,22 +572,22 @@
         <v>11</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
@@ -583,7 +601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
@@ -597,39 +615,123 @@
         <v>11</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>29</v>
+      <c r="D6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add hostname-prefixed logging feature
- Log files now automatically include hostname prefix for multi-machine identification
- Format: hostname-originalname.ext (e.g., LPRIME-excel-tool.log from excel-tool.log)
- Maintains directory structure and file extensions from original configuration
- Invalid filename characters in hostnames normalized to underscores
- Updated documentation with technical details and examples

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266B51A-63CA-4DF1-A2C1-0113B0BAA44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE572BE-0120-4412-9490-CAA95E29E9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -103,13 +103,7 @@
     <t>N\A</t>
   </si>
   <si>
-    <t>2025-09-09 21:04:44</t>
-  </si>
-  <si>
-    <t>2025-09-09 21:04:49</t>
-  </si>
-  <si>
-    <t>2025-09-09 21:40:41</t>
+    <t>2025-09-10 16:44:11</t>
   </si>
   <si>
     <t>Y</t>
@@ -124,9 +118,6 @@
     <t/>
   </si>
   <si>
-    <t>2025-09-09 21:40:42</t>
-  </si>
-  <si>
     <t>2025-08-23 22:39:06</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
   </si>
   <si>
     <t>UNC access denied - cannot determine file existence</t>
-  </si>
-  <si>
-    <t>2025-09-09 21:40:47</t>
   </si>
 </sst>
 </file>
@@ -512,7 +500,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E2" sqref="E2:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,19 +560,19 @@
         <v>11</v>
       </c>
       <c r="E2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -615,19 +603,19 @@
         <v>11</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -647,16 +635,16 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -673,10 +661,10 @@
         <v>11</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -693,16 +681,16 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -722,16 +710,16 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add configurable invalid path detection with detailed error messages
- Add invalid.path.detection setting (default: true) to enable/disable path validation
- Improve JAR filename validation to check only filename, not full path (fixes false positives for paths like C:\Program Files\...)
- Provide specific error messages for invalid paths instead of generic "X" marking
- Update documentation with new configuration option and validation details
- Enhanced error reporting shows exact reason for path rejection (e.g., "JAR filename contains spaces: file name.jar")

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample.xlsx
+++ b/sample-data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docs\Projects\Code\VulnAnalysisTool\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE572BE-0120-4412-9490-CAA95E29E9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C35E23-EA13-42AD-8C2D-BB851CED246C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="39">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -103,7 +103,10 @@
     <t>N\A</t>
   </si>
   <si>
-    <t>2025-09-10 16:44:11</t>
+    <t>C:\Program Files\BMC Software\Control-M Agent\Default\EXE_9.0.20.200\Jars\jackson-databind-2.10.3.jar</t>
+  </si>
+  <si>
+    <t>2025-09-10 21:32:19</t>
   </si>
   <si>
     <t>Y</t>
@@ -125,6 +128,24 @@
   </si>
   <si>
     <t>UNC access denied - cannot determine file existence</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2025-09-10 21:40:37</t>
+  </si>
+  <si>
+    <t>Path is a directory, not a file</t>
+  </si>
+  <si>
+    <t>Empty file path</t>
+  </si>
+  <si>
+    <t>Path marked as N/A</t>
+  </si>
+  <si>
+    <t>2025-09-10 21:53:58</t>
   </si>
 </sst>
 </file>
@@ -497,17 +518,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:L8"/>
+      <selection activeCell="E2" sqref="E2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="14.81640625"/>
     <col min="2" max="2" customWidth="true" width="22.08984375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="66.26953125"/>
+    <col min="3" max="3" customWidth="true" width="71.453125"/>
     <col min="4" max="4" customWidth="true" width="16.54296875"/>
     <col min="6" max="6" customWidth="true" width="20.7265625"/>
     <col min="7" max="7" customWidth="true" width="11.0"/>
@@ -560,19 +581,19 @@
         <v>11</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
+      <c r="H2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -603,19 +624,19 @@
         <v>11</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
+      <c r="G4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -634,17 +655,17 @@
       <c r="E5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
+      <c r="F5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -661,10 +682,10 @@
         <v>11</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -680,17 +701,17 @@
       <c r="E7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
+      <c r="F7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -709,17 +730,46 @@
       <c r="E8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="F8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>24</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>